<commit_message>
Archivos enviados por Eugenia Arce
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion04/ESCALETA_CS_07_04_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion04/ESCALETA_CS_07_04_CO.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\Ecaletas\Escaletas ajustadas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18375" windowHeight="6690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18375" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Escaleta03" sheetId="1" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="2" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta03!$P$1:$P$44</definedName>
-  </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="228">
   <si>
     <t>Asignatura</t>
   </si>
@@ -440,6 +442,9 @@
   </si>
   <si>
     <t>Las monarquías absolutas</t>
+  </si>
+  <si>
+    <t>RM_01_02_CO</t>
   </si>
   <si>
     <t>2º ESO</t>
@@ -678,6 +683,9 @@
     <t xml:space="preserve">La Reforma </t>
   </si>
   <si>
+    <t>Recurso M10A--01</t>
+  </si>
+  <si>
     <t xml:space="preserve">Actividad que permite identificar los actores y las relaciones involucradas en el conflicto religioso del siglo XVI el cual originó el movimiento social conocido como La Reforma </t>
   </si>
   <si>
@@ -687,6 +695,9 @@
     <t xml:space="preserve">Refuerza tu aprendizaje: La revolución científica y técnica </t>
   </si>
   <si>
+    <t>Recurso F1-01</t>
+  </si>
+  <si>
     <t>Recurso M13A-01</t>
   </si>
   <si>
@@ -696,34 +707,28 @@
     <t>Refuerza tu aprendizaje: El Estado moderno: el despotismo ilustrado</t>
   </si>
   <si>
+    <t>Recurso F 13-01</t>
+  </si>
+  <si>
+    <t>RF_01_02_CO</t>
+  </si>
+  <si>
+    <t>RF_01_03_CO</t>
+  </si>
+  <si>
+    <t>RM_01_03_CO</t>
+  </si>
+  <si>
+    <t>RM_01_04_CO</t>
+  </si>
+  <si>
+    <t>RF_01_04_CO</t>
+  </si>
+  <si>
     <t>RM_01_05_CO</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: El absolutismo en Europa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>Recurso M4A-01</t>
-  </si>
-  <si>
-    <t>Mapa Conceptual</t>
-  </si>
-  <si>
-    <t>M4a</t>
-  </si>
-  <si>
-    <t>Recurso M10A-01</t>
-  </si>
-  <si>
-    <t>Recurso F7-02</t>
-  </si>
-  <si>
-    <t>Recurso F13-01</t>
   </si>
 </sst>
 </file>
@@ -731,9 +736,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,12 +773,10 @@
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -786,12 +789,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -952,7 +949,7 @@
   </borders>
   <cellStyleXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1208,7 +1205,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1221,7 +1218,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,7 +1230,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1260,19 +1257,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1281,10 +1269,16 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1819,7 +1813,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1827,11 +1821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1850,8 +1843,8 @@
     <col min="12" max="12" width="16.140625" style="6" customWidth="1"/>
     <col min="13" max="13" width="10.140625" style="6" customWidth="1"/>
     <col min="14" max="14" width="8.28515625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="4" style="6" customWidth="1"/>
+    <col min="15" max="15" width="31" style="6" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="6" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" style="6" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" style="6" customWidth="1"/>
     <col min="19" max="19" width="45.28515625" style="6" customWidth="1"/>
@@ -1861,94 +1854,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22" t="s">
+      <c r="N1" s="21"/>
+      <c r="O1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="U1" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" ht="8.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
+    <row r="2" spans="1:21" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
       <c r="M2" s="9" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="25"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="28"/>
     </row>
     <row r="3" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1961,12 +1954,12 @@
         <v>94</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H3" s="13">
         <v>1</v>
@@ -1975,7 +1968,7 @@
         <v>95</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>69</v>
@@ -1988,7 +1981,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>96</v>
@@ -2003,7 +1996,7 @@
         <v>129</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="U3" s="17" t="s">
         <v>130</v>
@@ -2020,10 +2013,10 @@
         <v>94</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="13" t="s">
@@ -2036,7 +2029,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>70</v>
@@ -2077,10 +2070,10 @@
         <v>94</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="13" t="s">
@@ -2117,7 +2110,7 @@
         <v>98</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="U5" s="17" t="s">
         <v>99</v>
@@ -2134,10 +2127,10 @@
         <v>94</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="13" t="s">
@@ -2150,7 +2143,7 @@
         <v>92</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>70</v>
@@ -2191,7 +2184,7 @@
         <v>94</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -2229,7 +2222,7 @@
         <v>98</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="U7" s="17" t="s">
         <v>99</v>
@@ -2246,14 +2239,14 @@
         <v>94</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H8" s="13">
         <v>6</v>
@@ -2262,7 +2255,7 @@
         <v>92</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>69</v>
@@ -2275,7 +2268,7 @@
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="15" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>96</v>
@@ -2290,7 +2283,7 @@
         <v>132</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="U8" s="17" t="s">
         <v>133</v>
@@ -2307,10 +2300,10 @@
         <v>94</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="s">
@@ -2364,10 +2357,10 @@
         <v>94</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="13" t="s">
@@ -2421,10 +2414,10 @@
         <v>94</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="13" t="s">
@@ -2437,7 +2430,7 @@
         <v>92</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>70</v>
@@ -2478,7 +2471,7 @@
         <v>94</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2492,7 +2485,7 @@
         <v>95</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>69</v>
@@ -2505,7 +2498,7 @@
         <v>38</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="P12" s="15" t="s">
         <v>19</v>
@@ -2523,10 +2516,10 @@
         <v>135</v>
       </c>
       <c r="U12" s="17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>66</v>
       </c>
@@ -2537,10 +2530,10 @@
         <v>94</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="13"/>
@@ -2559,7 +2552,7 @@
       <c r="T13" s="16"/>
       <c r="U13" s="17"/>
     </row>
-    <row r="14" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>66</v>
       </c>
@@ -2570,11 +2563,11 @@
         <v>94</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2592,7 +2585,7 @@
       <c r="T14" s="16"/>
       <c r="U14" s="17"/>
     </row>
-    <row r="15" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>66</v>
       </c>
@@ -2603,11 +2596,11 @@
         <v>94</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -2625,7 +2618,7 @@
       <c r="T15" s="16"/>
       <c r="U15" s="17"/>
     </row>
-    <row r="16" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>66</v>
       </c>
@@ -2636,11 +2629,11 @@
         <v>94</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -2669,14 +2662,14 @@
         <v>94</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H17" s="13">
         <v>11</v>
@@ -2685,7 +2678,7 @@
         <v>92</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K17" s="15" t="s">
         <v>69</v>
@@ -2713,10 +2706,10 @@
         <v>132</v>
       </c>
       <c r="T17" s="16" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="U17" s="17" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2730,14 +2723,14 @@
         <v>94</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="13" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H18" s="13">
         <v>12</v>
@@ -2746,7 +2739,7 @@
         <v>95</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K18" s="15" t="s">
         <v>70</v>
@@ -2787,7 +2780,7 @@
         <v>94</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -2801,7 +2794,7 @@
         <v>95</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K19" s="15" t="s">
         <v>69</v>
@@ -2814,7 +2807,7 @@
         <v>34</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="P19" s="15" t="s">
         <v>96</v>
@@ -2829,10 +2822,10 @@
         <v>129</v>
       </c>
       <c r="T19" s="16" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U19" s="17" t="s">
-        <v>130</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2846,14 +2839,14 @@
         <v>94</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H20" s="13">
         <v>14</v>
@@ -2862,7 +2855,7 @@
         <v>92</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K20" s="15" t="s">
         <v>69</v>
@@ -2875,7 +2868,7 @@
       </c>
       <c r="N20" s="15"/>
       <c r="O20" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P20" s="15" t="s">
         <v>19</v>
@@ -2890,10 +2883,10 @@
         <v>132</v>
       </c>
       <c r="T20" s="16" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="U20" s="17" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2907,14 +2900,14 @@
         <v>94</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H21" s="13">
         <v>15</v>
@@ -2923,7 +2916,7 @@
         <v>92</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>70</v>
@@ -2947,13 +2940,13 @@
         <v>115</v>
       </c>
       <c r="T21" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="U21" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>66</v>
       </c>
@@ -2964,10 +2957,10 @@
         <v>94</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="13"/>
@@ -2986,7 +2979,7 @@
       <c r="T22" s="16"/>
       <c r="U22" s="17"/>
     </row>
-    <row r="23" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>66</v>
       </c>
@@ -2997,13 +2990,13 @@
         <v>94</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
@@ -3021,7 +3014,7 @@
       <c r="T23" s="16"/>
       <c r="U23" s="17"/>
     </row>
-    <row r="24" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>66</v>
       </c>
@@ -3032,13 +3025,13 @@
         <v>94</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -3067,10 +3060,10 @@
         <v>94</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="13" t="s">
@@ -3083,7 +3076,7 @@
         <v>96</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>70</v>
@@ -3098,7 +3091,7 @@
         <v>19</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R25" s="16" t="s">
         <v>91</v>
@@ -3124,14 +3117,14 @@
         <v>94</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="13" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="H26" s="13">
         <v>17</v>
@@ -3140,7 +3133,7 @@
         <v>92</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K26" s="15" t="s">
         <v>70</v>
@@ -3181,7 +3174,7 @@
         <v>94</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -3236,14 +3229,14 @@
         <v>94</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H28" s="13">
         <v>19</v>
@@ -3252,7 +3245,7 @@
         <v>92</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>69</v>
@@ -3265,7 +3258,7 @@
       </c>
       <c r="N28" s="15"/>
       <c r="O28" s="15" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="P28" s="15" t="s">
         <v>19</v>
@@ -3280,13 +3273,13 @@
         <v>132</v>
       </c>
       <c r="T28" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="U28" s="17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="U28" s="19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>66</v>
       </c>
@@ -3297,15 +3290,13 @@
         <v>94</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F29" s="11"/>
-      <c r="G29" s="13" t="s">
-        <v>219</v>
-      </c>
+      <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -3321,7 +3312,7 @@
       <c r="T29" s="16"/>
       <c r="U29" s="19"/>
     </row>
-    <row r="30" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>66</v>
       </c>
@@ -3332,13 +3323,13 @@
         <v>94</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
@@ -3356,7 +3347,7 @@
       <c r="T30" s="16"/>
       <c r="U30" s="19"/>
     </row>
-    <row r="31" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>66</v>
       </c>
@@ -3367,13 +3358,13 @@
         <v>94</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
@@ -3402,10 +3393,10 @@
         <v>94</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="13" t="s">
@@ -3418,7 +3409,7 @@
         <v>92</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K32" s="15" t="s">
         <v>70</v>
@@ -3459,7 +3450,7 @@
         <v>94</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -3488,7 +3479,7 @@
         <v>19</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R33" s="18" t="s">
         <v>91</v>
@@ -3514,10 +3505,10 @@
         <v>94</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="13" t="s">
@@ -3571,14 +3562,14 @@
         <v>94</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="13" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H35" s="13">
         <v>23</v>
@@ -3587,7 +3578,7 @@
         <v>92</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K35" s="15" t="s">
         <v>70</v>
@@ -3628,12 +3619,12 @@
         <v>94</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H36" s="13">
         <v>24</v>
@@ -3642,7 +3633,7 @@
         <v>96</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K36" s="15" t="s">
         <v>69</v>
@@ -3655,7 +3646,7 @@
         <v>45</v>
       </c>
       <c r="O36" s="15" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="P36" s="15" t="s">
         <v>19</v>
@@ -3670,10 +3661,10 @@
         <v>129</v>
       </c>
       <c r="T36" s="16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="U36" s="19" t="s">
-        <v>130</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3687,12 +3678,12 @@
         <v>94</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H37" s="13">
         <v>25</v>
@@ -3701,7 +3692,7 @@
         <v>92</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K37" s="15" t="s">
         <v>70</v>
@@ -3716,7 +3707,7 @@
         <v>19</v>
       </c>
       <c r="Q37" s="18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="R37" s="18" t="s">
         <v>91</v>
@@ -3725,7 +3716,7 @@
         <v>123</v>
       </c>
       <c r="T37" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="U37" s="19" t="s">
         <v>125</v>
@@ -3742,31 +3733,25 @@
         <v>94</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H38" s="13">
         <v>26</v>
       </c>
       <c r="I38" s="13"/>
-      <c r="J38" s="13" t="s">
-        <v>222</v>
-      </c>
+      <c r="J38" s="13"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
-      <c r="P38" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q38" s="16" t="s">
-        <v>219</v>
-      </c>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
       <c r="S38" s="16"/>
       <c r="T38" s="16"/>
@@ -3783,12 +3768,12 @@
         <v>94</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H39" s="13">
         <v>27</v>
@@ -3797,7 +3782,7 @@
         <v>92</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K39" s="15" t="s">
         <v>70</v>
@@ -3806,30 +3791,28 @@
         <v>32</v>
       </c>
       <c r="M39" s="15"/>
-      <c r="N39" s="15" t="s">
-        <v>223</v>
-      </c>
+      <c r="N39" s="15"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q39" s="18">
-        <v>6</v>
-      </c>
-      <c r="R39" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="S39" s="16" t="s">
-        <v>132</v>
+      <c r="Q39" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="R39" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="S39" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="T39" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="U39" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="U39" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>66</v>
       </c>
@@ -3840,12 +3823,12 @@
         <v>94</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H40" s="13">
         <v>28</v>
@@ -3854,7 +3837,7 @@
         <v>92</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K40" s="15" t="s">
         <v>69</v>
@@ -3867,7 +3850,7 @@
       </c>
       <c r="N40" s="15"/>
       <c r="O40" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="P40" s="15" t="s">
         <v>20</v>
@@ -3882,30 +3865,21 @@
         <v>132</v>
       </c>
       <c r="T40" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="U40" s="16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="G44" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="P44" s="21"/>
+        <v>226</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="P1:P44">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Si"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
@@ -3919,13 +3893,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3943,7 +3910,7 @@
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M18:M39 M3:M16 N39</xm:sqref>
+          <xm:sqref>M18:M39 M3:M16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3961,7 +3928,7 @@
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N38</xm:sqref>
+          <xm:sqref>N3:N39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>